<commit_message>
Added in scout scan (skip data saving) option updated requirment document to correct typos
</commit_message>
<xml_diff>
--- a/SoftwareRequirement/User interface specification.xlsx
+++ b/SoftwareRequirement/User interface specification.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcuFLSA\Documents\GitRepo\FLSLV\SoftwareRequirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A36EB0E8-25A1-4EBB-8001-424CD99E1904}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE9E4F3-EA7F-42F5-A1ED-9D5B01E67136}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Software Specification" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="160">
   <si>
     <t>Area</t>
   </si>
@@ -263,9 +263,6 @@
     <t>Priority(Low, Med. High)</t>
   </si>
   <si>
-    <t>Med</t>
-  </si>
-  <si>
     <t>Low</t>
   </si>
   <si>
@@ -326,9 +323,6 @@
     <t>Use - Chime</t>
   </si>
   <si>
-    <t>Hihg</t>
-  </si>
-  <si>
     <t>Text</t>
   </si>
   <si>
@@ -360,9 +354,6 @@
   </si>
   <si>
     <t>Parameter to show system health status based on refrence</t>
-  </si>
-  <si>
-    <t>HIgh</t>
   </si>
   <si>
     <t>Stop system if single point failure of the laser is detected</t>
@@ -416,9 +407,6 @@
     <t>REQ6</t>
   </si>
   <si>
-    <t>REQ7</t>
-  </si>
-  <si>
     <t>REQ8</t>
   </si>
   <si>
@@ -453,12 +441,6 @@
   </si>
   <si>
     <t>REQ19</t>
-  </si>
-  <si>
-    <t>REQ20</t>
-  </si>
-  <si>
-    <t>REQ21</t>
   </si>
   <si>
     <t>REQ22</t>
@@ -525,6 +507,9 @@
   </si>
   <si>
     <t>Count(for sorting)</t>
+  </si>
+  <si>
+    <t>Medium</t>
   </si>
 </sst>
 </file>
@@ -1053,9 +1038,9 @@
   </sheetPr>
   <dimension ref="A1:AC999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1080,7 +1065,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>76</v>
@@ -1101,7 +1086,7 @@
         <v>1</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -1125,10 +1110,10 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>33</v>
@@ -1137,7 +1122,7 @@
         <v>75</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>34</v>
@@ -1176,10 +1161,10 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>35</v>
@@ -1188,7 +1173,7 @@
         <v>75</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>36</v>
@@ -1225,10 +1210,10 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>39</v>
@@ -1237,7 +1222,7 @@
         <v>75</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>40</v>
@@ -1276,19 +1261,19 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>19</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>20</v>
@@ -1327,7 +1312,7 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>71</v>
@@ -1339,7 +1324,7 @@
         <v>75</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>7</v>
@@ -1378,19 +1363,19 @@
     </row>
     <row r="7" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>77</v>
+        <v>159</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>46</v>
@@ -1426,20 +1411,20 @@
       <c r="AC7" s="4"/>
     </row>
     <row r="8" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>128</v>
+      <c r="A8" s="8">
+        <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>50</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>77</v>
+        <v>159</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>51</v>
@@ -1476,19 +1461,19 @@
     </row>
     <row r="9" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>52</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>53</v>
@@ -1525,10 +1510,10 @@
     </row>
     <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>22</v>
@@ -1537,7 +1522,7 @@
         <v>75</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>23</v>
@@ -1574,10 +1559,10 @@
     </row>
     <row r="11" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>24</v>
@@ -1586,7 +1571,7 @@
         <v>75</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>25</v>
@@ -1625,10 +1610,10 @@
     </row>
     <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>26</v>
@@ -1637,7 +1622,7 @@
         <v>75</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>27</v>
@@ -1676,10 +1661,10 @@
     </row>
     <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>29</v>
@@ -1688,7 +1673,7 @@
         <v>75</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>30</v>
@@ -1727,10 +1712,10 @@
     </row>
     <row r="14" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" s="10" t="s">
         <v>31</v>
@@ -1739,7 +1724,7 @@
         <v>75</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>32</v>
@@ -1778,19 +1763,19 @@
     </row>
     <row r="15" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3" t="s">
@@ -1827,22 +1812,22 @@
     </row>
     <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>75</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>8</v>
@@ -1876,10 +1861,10 @@
     </row>
     <row r="17" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>47</v>
@@ -1888,7 +1873,7 @@
         <v>75</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>48</v>
@@ -1925,10 +1910,10 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>37</v>
@@ -1937,7 +1922,7 @@
         <v>75</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>38</v>
@@ -1976,19 +1961,19 @@
     </row>
     <row r="19" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>49</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F19" s="4"/>
       <c r="G19" s="3"/>
@@ -2021,10 +2006,10 @@
     </row>
     <row r="20" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>17</v>
@@ -2033,7 +2018,7 @@
         <v>75</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>18</v>
@@ -2071,8 +2056,8 @@
       <c r="AC20" s="4"/>
     </row>
     <row r="21" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>141</v>
+      <c r="A21" s="8">
+        <v>20</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>72</v>
@@ -2081,10 +2066,10 @@
         <v>11</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>12</v>
@@ -2122,11 +2107,11 @@
       <c r="AC21" s="4"/>
     </row>
     <row r="22" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>142</v>
+      <c r="A22" s="8">
+        <v>21</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>21</v>
@@ -2135,7 +2120,7 @@
         <v>75</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F22" s="4"/>
       <c r="G22" s="4" t="s">
@@ -2172,7 +2157,7 @@
     </row>
     <row r="23" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>73</v>
@@ -2184,7 +2169,7 @@
         <v>75</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>14</v>
@@ -2223,7 +2208,7 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>74</v>
@@ -2232,10 +2217,10 @@
         <v>15</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>77</v>
+        <v>159</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>16</v>
@@ -2272,19 +2257,19 @@
     </row>
     <row r="25" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>77</v>
+        <v>159</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>10</v>
@@ -2323,22 +2308,22 @@
     </row>
     <row r="26" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C26" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>106</v>
-      </c>
       <c r="F26" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>8</v>
@@ -2374,22 +2359,22 @@
     </row>
     <row r="27" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>8</v>
@@ -2425,28 +2410,28 @@
     </row>
     <row r="28" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D28" s="4" t="s">
         <v>75</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I28" s="4" t="s">
         <v>5</v>
@@ -2476,28 +2461,28 @@
     </row>
     <row r="29" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D29" s="4" t="s">
         <v>75</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I29" s="4" t="s">
         <v>5</v>
@@ -2527,28 +2512,28 @@
     </row>
     <row r="30" spans="1:29" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>75</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="G30" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I30" s="4" t="s">
         <v>5</v>
@@ -2578,28 +2563,28 @@
     </row>
     <row r="31" spans="1:29" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>77</v>
+        <v>159</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H31" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>5</v>
@@ -31723,13 +31708,13 @@
   <sheetData>
     <row r="1" spans="1:29" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>76</v>
@@ -31775,7 +31760,7 @@
         <v>27</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>43</v>
@@ -31784,7 +31769,7 @@
         <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>44</v>
@@ -31796,7 +31781,7 @@
         <v>28</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>41</v>
@@ -31805,7 +31790,7 @@
         <v>75</v>
       </c>
       <c r="E3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>42</v>
@@ -31823,7 +31808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70D7AE29-BBAD-4379-8DE1-22F2C1D3C58F}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
@@ -31850,7 +31835,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D1" s="16" t="s">
         <v>76</v>
@@ -31871,7 +31856,7 @@
         <v>1</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
@@ -31895,22 +31880,22 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>75</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G2" s="17" t="s">
         <v>8</v>
@@ -31924,22 +31909,22 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D3" s="17" t="s">
         <v>75</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G3" s="17" t="s">
         <v>8</v>

</xml_diff>